<commit_message>
updating part2 cleaning to reflect new columns and utting individual class assertions for each column
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B41D44-76EC-0A43-8AAA-F4BC3AD67CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF32AC0-30B7-3345-8E39-6037AC0339EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2972,9 +2972,6 @@
     <t>in shade</t>
   </si>
   <si>
-    <t>vCoodUncM</t>
-  </si>
-  <si>
     <t>Rumex</t>
   </si>
   <si>
@@ -3078,6 +3075,9 @@
   </si>
   <si>
     <t>assCollTaxa</t>
+  </si>
+  <si>
+    <t>vCoordUncM</t>
   </si>
 </sst>
 </file>
@@ -3559,7 +3559,7 @@
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3601,43 +3601,43 @@
   <sheetData>
     <row r="1" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>4</v>
@@ -3652,7 +3652,7 @@
         <v>12</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>5</v>
@@ -3664,31 +3664,31 @@
         <v>19</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="Y1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>7</v>
@@ -3732,7 +3732,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>16</v>
@@ -3750,7 +3750,7 @@
         <v>21</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>18</v>
@@ -3792,7 +3792,7 @@
         <v>14</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>16</v>
@@ -3848,7 +3848,7 @@
         <v>14</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>16</v>
@@ -3898,7 +3898,7 @@
         <v>14</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>16</v>
@@ -3952,7 +3952,7 @@
         <v>14</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>16</v>
@@ -4006,7 +4006,7 @@
         <v>14</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>16</v>
@@ -4056,7 +4056,7 @@
         <v>14</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>16</v>
@@ -4110,7 +4110,7 @@
         <v>14</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>16</v>
@@ -4161,7 +4161,7 @@
         <v>14</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>16</v>
@@ -4215,7 +4215,7 @@
         <v>14</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>16</v>
@@ -4270,7 +4270,7 @@
         <v>14</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>16</v>
@@ -4282,7 +4282,7 @@
         <v>67</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>11</v>
@@ -4291,7 +4291,7 @@
         <v>71</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>18</v>
@@ -4333,7 +4333,7 @@
         <v>14</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>16</v>
@@ -4392,7 +4392,7 @@
         <v>14</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>16</v>
@@ -4447,7 +4447,7 @@
         <v>14</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>16</v>
@@ -4502,7 +4502,7 @@
         <v>14</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>16</v>
@@ -4557,7 +4557,7 @@
         <v>14</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>16</v>
@@ -4612,7 +4612,7 @@
         <v>14</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>16</v>
@@ -4667,7 +4667,7 @@
         <v>14</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>16</v>
@@ -4722,7 +4722,7 @@
         <v>14</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>16</v>
@@ -4777,7 +4777,7 @@
         <v>14</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>16</v>
@@ -4832,7 +4832,7 @@
         <v>14</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>16</v>
@@ -4887,7 +4887,7 @@
         <v>14</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>16</v>
@@ -4921,13 +4921,13 @@
         <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H24" s="4">
         <v>20040312</v>
@@ -4942,7 +4942,7 @@
         <v>14</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>16</v>
@@ -4999,7 +4999,7 @@
         <v>14</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>16</v>
@@ -5054,7 +5054,7 @@
         <v>14</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>16</v>
@@ -5085,16 +5085,16 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" t="s">
         <v>147</v>
-      </c>
-      <c r="E27" t="s">
-        <v>148</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H27" s="4">
         <v>20040312</v>
@@ -5109,7 +5109,7 @@
         <v>14</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>16</v>
@@ -5118,7 +5118,7 @@
         <v>8</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P27"/>
       <c r="Q27" s="4" t="s">
@@ -5164,7 +5164,7 @@
         <v>14</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>16</v>
@@ -5182,7 +5182,7 @@
         <v>18</v>
       </c>
       <c r="AF28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -5220,7 +5220,7 @@
         <v>14</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>16</v>
@@ -5238,7 +5238,7 @@
         <v>18</v>
       </c>
       <c r="AF29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -5276,7 +5276,7 @@
         <v>14</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>16</v>
@@ -5294,7 +5294,7 @@
         <v>18</v>
       </c>
       <c r="AF30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -5332,7 +5332,7 @@
         <v>14</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>16</v>
@@ -5353,7 +5353,7 @@
         <v>18</v>
       </c>
       <c r="AF31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5391,7 +5391,7 @@
         <v>14</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>16</v>
@@ -5441,7 +5441,7 @@
         <v>14</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>16</v>
@@ -5491,7 +5491,7 @@
         <v>14</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>16</v>
@@ -5544,7 +5544,7 @@
         <v>14</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>16</v>
@@ -5597,7 +5597,7 @@
         <v>14</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>16</v>
@@ -5650,7 +5650,7 @@
         <v>14</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>16</v>
@@ -5700,7 +5700,7 @@
         <v>14</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>16</v>
@@ -5750,7 +5750,7 @@
         <v>14</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>16</v>
@@ -5800,7 +5800,7 @@
         <v>14</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>16</v>
@@ -5850,7 +5850,7 @@
         <v>14</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>16</v>
@@ -5900,7 +5900,7 @@
         <v>14</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>16</v>
@@ -5950,7 +5950,7 @@
         <v>14</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>16</v>
@@ -6000,7 +6000,7 @@
         <v>14</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>16</v>
@@ -6050,7 +6050,7 @@
         <v>14</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>16</v>
@@ -6100,7 +6100,7 @@
         <v>14</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>16</v>
@@ -6150,7 +6150,7 @@
         <v>14</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>16</v>
@@ -6159,7 +6159,7 @@
         <v>8</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P47" s="4" t="s">
         <v>130</v>
@@ -6171,7 +6171,7 @@
         <v>18</v>
       </c>
       <c r="AF47" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -6209,7 +6209,7 @@
         <v>14</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>16</v>
@@ -6262,7 +6262,7 @@
         <v>14</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>16</v>
@@ -6315,7 +6315,7 @@
         <v>14</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>16</v>
@@ -6368,7 +6368,7 @@
         <v>14</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M51" s="4" t="s">
         <v>16</v>
@@ -6421,7 +6421,7 @@
         <v>14</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M52" s="4" t="s">
         <v>16</v>
@@ -6474,7 +6474,7 @@
         <v>14</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>16</v>
@@ -6527,7 +6527,7 @@
         <v>14</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>16</v>
@@ -6580,7 +6580,7 @@
         <v>14</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>16</v>
@@ -6633,7 +6633,7 @@
         <v>14</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>16</v>
@@ -6686,7 +6686,7 @@
         <v>14</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>16</v>
@@ -6739,7 +6739,7 @@
         <v>14</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>16</v>
@@ -6757,7 +6757,7 @@
         <v>18</v>
       </c>
       <c r="AF58" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:32" ht="34" x14ac:dyDescent="0.2">
@@ -6795,7 +6795,7 @@
         <v>14</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>16</v>
@@ -6848,7 +6848,7 @@
         <v>14</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>16</v>
@@ -6901,7 +6901,7 @@
         <v>14</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>16</v>
@@ -6954,7 +6954,7 @@
         <v>14</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>16</v>
@@ -7007,7 +7007,7 @@
         <v>14</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>16</v>
@@ -7036,16 +7036,16 @@
         <v>30</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H64" s="4">
         <v>20040312</v>
@@ -7060,7 +7060,7 @@
         <v>14</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
updating occurrence data entry protocol
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD33E8E-9A80-134D-8888-33088492533E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEF351-991D-FC46-8585-B0D959865859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -1348,33 +1348,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{B9586400-66D1-7141-8F4F-DF928AA236E2}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">locationRemarks
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">assOcc
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1400,33 +1387,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: poly 20
-</t>
+          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"HJC-2863"</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C334D07E-4730-1749-B76E-5A26B42DC1C1}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
       <text>
         <r>
           <rPr>
@@ -1436,7 +1431,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vTaxonRank (REQUIRED)
+          <t xml:space="preserve">assTaxa
 </t>
         </r>
         <r>
@@ -1478,7 +1473,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">verbatim taxon rank. The lowest level of taxonomy provided. 
+          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
 </t>
         </r>
         <r>
@@ -1508,22 +1503,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">if specific epiphet in scientific name = "species", alternatively if lowest level is generic name = "genus"
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>Isoetes echinospora</t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{CA3A2C45-C583-DA43-877C-3A38B460B025}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{B9586400-66D1-7141-8F4F-DF928AA236E2}">
       <text>
         <r>
           <rPr>
@@ -1533,30 +1517,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>vElev</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">locationRemarks
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1582,389 +1559,423 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: 10 </t>
+          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: poly 20
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{9F8D95FB-54D3-F04C-9134-F2DD1CEAD6ED}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{C334D07E-4730-1749-B76E-5A26B42DC1C1}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vLat 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>49 39 12</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vTaxonRank (REQUIRED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">verbatim taxon rank. The lowest level of taxonomy provided. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if specific epiphet in scientific name = "species", alternatively if lowest level is generic name = "genus"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{A76DD89C-13AB-F048-A935-8FD1A912F16A}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{CA3A2C45-C583-DA43-877C-3A38B460B025}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">RECOMMENDED
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>vElev</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: 10 </t>
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{B3BFE285-5D7E-014B-96D5-A3177370E856}">
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{9F8D95FB-54D3-F04C-9134-F2DD1CEAD6ED}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vUTM
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>10U 45689 55678</t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vLat 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>49 39 12</t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{C36EAF92-CB2B-8247-A6B4-E6839E892AD6}">
+    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{A76DD89C-13AB-F048-A935-8FD1A912F16A}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">vCoordUncertainty
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">30 </t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">RECOMMENDED
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{B3BFE285-5D7E-014B-96D5-A3177370E856}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assOcc
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vUTM
 </t>
         </r>
         <r>
@@ -1994,7 +2005,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
+          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
 </t>
         </r>
         <r>
@@ -2024,11 +2035,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>"HJC-2863"</t>
+          <t>10U 45689 55678</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{C36EAF92-CB2B-8247-A6B4-E6839E892AD6}">
       <text>
         <r>
           <rPr>
@@ -2038,18 +2049,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">assTaxa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">vCoordUncertainty
 </t>
         </r>
         <r>
@@ -2080,7 +2080,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
+          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
 </t>
         </r>
         <r>
@@ -2110,7 +2110,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Isoetes echinospora</t>
+          <t xml:space="preserve">30 </t>
         </r>
       </text>
     </comment>
@@ -2475,7 +2475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="181">
   <si>
     <t>genus</t>
   </si>
@@ -2957,9 +2957,6 @@
     <t>orgQtype</t>
   </si>
   <si>
-    <t>individuals</t>
-  </si>
-  <si>
     <t>phenology</t>
   </si>
   <si>
@@ -3012,6 +3009,15 @@
   </si>
   <si>
     <t>idQualifier</t>
+  </si>
+  <si>
+    <t>qualitative</t>
+  </si>
+  <si>
+    <t>few</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -3497,10 +3503,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3520,15 +3526,15 @@
     <col min="13" max="13" width="20.33203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="4"/>
     <col min="15" max="15" width="22.1640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.83203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.83203125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="8.5" style="4" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="29.5" style="4" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="29.5" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.83203125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="8.5" style="4" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" style="4" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="4" customWidth="1"/>
     <col min="25" max="25" width="7.5" style="4" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="4" customWidth="1"/>
     <col min="27" max="27" width="11.1640625" style="4" customWidth="1"/>
@@ -3542,40 +3548,40 @@
   <sheetData>
     <row r="1" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="L1" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>150</v>
@@ -3586,29 +3592,29 @@
       <c r="O1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>176</v>
@@ -3626,7 +3632,7 @@
         <v>20</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>153</v>
@@ -3670,7 +3676,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L2"/>
       <c r="M2" s="4" t="s">
@@ -3679,17 +3685,17 @@
       <c r="N2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2"/>
+      <c r="S2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U2"/>
-      <c r="V2"/>
+      <c r="W2"/>
       <c r="X2"/>
       <c r="Z2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>18</v>
@@ -3728,7 +3734,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L3"/>
       <c r="M3" s="4" t="s">
@@ -3740,11 +3746,11 @@
       <c r="O3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U3"/>
-      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
       <c r="AD3" s="4" t="s">
         <v>18</v>
       </c>
@@ -3782,7 +3788,7 @@
         <v>14</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L4"/>
       <c r="M4" s="4" t="s">
@@ -3791,7 +3797,7 @@
       <c r="N4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD4" s="4" t="s">
@@ -3830,7 +3836,7 @@
         <v>14</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L5"/>
       <c r="M5" s="4" t="s">
@@ -3842,7 +3848,7 @@
       <c r="O5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD5" s="4" t="s">
@@ -3882,7 +3888,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L6"/>
       <c r="M6" s="4" t="s">
@@ -3894,7 +3900,10 @@
       <c r="O6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="R6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD6" s="4" t="s">
@@ -3934,7 +3943,7 @@
         <v>14</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L7"/>
       <c r="M7" s="4" t="s">
@@ -3943,7 +3952,7 @@
       <c r="N7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD7" s="4" t="s">
@@ -3982,7 +3991,7 @@
         <v>14</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L8"/>
       <c r="M8" s="4" t="s">
@@ -3994,7 +4003,7 @@
       <c r="O8" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD8" s="4" t="s">
@@ -4034,7 +4043,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L9"/>
       <c r="M9" s="4" t="s">
@@ -4043,7 +4052,7 @@
       <c r="N9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD9" s="4" t="s">
@@ -4083,7 +4092,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L10"/>
       <c r="M10" s="4" t="s">
@@ -4095,7 +4104,7 @@
       <c r="O10" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD10" s="4" t="s">
@@ -4135,7 +4144,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L11"/>
       <c r="M11" s="4" t="s">
@@ -4147,8 +4156,8 @@
       <c r="O11" t="s">
         <v>67</v>
       </c>
-      <c r="P11"/>
-      <c r="Q11" s="4" t="s">
+      <c r="R11"/>
+      <c r="S11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD11" s="4" t="s">
@@ -4188,7 +4197,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L12"/>
       <c r="M12" s="4" t="s">
@@ -4200,17 +4209,17 @@
       <c r="O12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="S12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Z12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>18</v>
@@ -4249,7 +4258,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L13"/>
       <c r="M13" s="4" t="s">
@@ -4261,8 +4270,8 @@
       <c r="O13" t="s">
         <v>67</v>
       </c>
-      <c r="P13"/>
-      <c r="Q13" s="4" t="s">
+      <c r="R13"/>
+      <c r="S13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AB13" t="s">
@@ -4306,7 +4315,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L14"/>
       <c r="M14" s="4" t="s">
@@ -4318,8 +4327,8 @@
       <c r="O14" t="s">
         <v>67</v>
       </c>
-      <c r="P14"/>
-      <c r="Q14" s="4" t="s">
+      <c r="R14"/>
+      <c r="S14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD14" s="4" t="s">
@@ -4359,7 +4368,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L15"/>
       <c r="M15" s="4" t="s">
@@ -4371,8 +4380,8 @@
       <c r="O15" t="s">
         <v>67</v>
       </c>
-      <c r="P15"/>
-      <c r="Q15" s="4" t="s">
+      <c r="R15"/>
+      <c r="S15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD15" s="4" t="s">
@@ -4412,7 +4421,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L16"/>
       <c r="M16" s="4" t="s">
@@ -4424,8 +4433,8 @@
       <c r="O16" t="s">
         <v>67</v>
       </c>
-      <c r="P16"/>
-      <c r="Q16" s="4" t="s">
+      <c r="R16"/>
+      <c r="S16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD16" s="4" t="s">
@@ -4465,7 +4474,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L17"/>
       <c r="M17" s="4" t="s">
@@ -4477,8 +4486,8 @@
       <c r="O17" t="s">
         <v>67</v>
       </c>
-      <c r="P17"/>
-      <c r="Q17" s="4" t="s">
+      <c r="R17"/>
+      <c r="S17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD17" s="4" t="s">
@@ -4518,7 +4527,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L18"/>
       <c r="M18" s="4" t="s">
@@ -4530,8 +4539,8 @@
       <c r="O18" t="s">
         <v>67</v>
       </c>
-      <c r="P18"/>
-      <c r="Q18" s="4" t="s">
+      <c r="R18"/>
+      <c r="S18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD18" s="4" t="s">
@@ -4571,7 +4580,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L19"/>
       <c r="M19" s="4" t="s">
@@ -4583,8 +4592,8 @@
       <c r="O19" t="s">
         <v>67</v>
       </c>
-      <c r="P19"/>
-      <c r="Q19" s="4" t="s">
+      <c r="R19"/>
+      <c r="S19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD19" s="4" t="s">
@@ -4624,7 +4633,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L20"/>
       <c r="M20" s="4" t="s">
@@ -4636,8 +4645,8 @@
       <c r="O20" t="s">
         <v>67</v>
       </c>
-      <c r="P20"/>
-      <c r="Q20" s="4" t="s">
+      <c r="R20"/>
+      <c r="S20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD20" s="4" t="s">
@@ -4677,7 +4686,7 @@
         <v>14</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L21"/>
       <c r="M21" s="4" t="s">
@@ -4689,8 +4698,8 @@
       <c r="O21" t="s">
         <v>67</v>
       </c>
-      <c r="P21"/>
-      <c r="Q21" s="4" t="s">
+      <c r="R21"/>
+      <c r="S21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD21" s="4" t="s">
@@ -4730,7 +4739,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L22"/>
       <c r="M22" s="4" t="s">
@@ -4742,8 +4751,8 @@
       <c r="O22" t="s">
         <v>67</v>
       </c>
-      <c r="P22"/>
-      <c r="Q22" s="4" t="s">
+      <c r="R22"/>
+      <c r="S22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD22" s="4" t="s">
@@ -4783,7 +4792,7 @@
         <v>14</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L23"/>
       <c r="M23" s="4" t="s">
@@ -4795,8 +4804,8 @@
       <c r="O23" t="s">
         <v>67</v>
       </c>
-      <c r="P23"/>
-      <c r="Q23" s="4" t="s">
+      <c r="R23"/>
+      <c r="S23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD23" s="4" t="s">
@@ -4836,7 +4845,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L24"/>
       <c r="M24" s="4" t="s">
@@ -4848,8 +4857,8 @@
       <c r="O24" t="s">
         <v>68</v>
       </c>
-      <c r="P24"/>
-      <c r="Q24" s="4" t="s">
+      <c r="R24"/>
+      <c r="S24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD24" s="4" t="s">
@@ -4891,7 +4900,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L25"/>
       <c r="M25" s="4" t="s">
@@ -4903,8 +4912,8 @@
       <c r="O25" t="s">
         <v>68</v>
       </c>
-      <c r="P25"/>
-      <c r="Q25" s="4" t="s">
+      <c r="R25"/>
+      <c r="S25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD25" s="4" t="s">
@@ -4944,7 +4953,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L26"/>
       <c r="M26" s="4" t="s">
@@ -4956,8 +4965,8 @@
       <c r="O26" t="s">
         <v>69</v>
       </c>
-      <c r="P26"/>
-      <c r="Q26" s="4" t="s">
+      <c r="R26"/>
+      <c r="S26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD26" s="4" t="s">
@@ -4997,7 +5006,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L27"/>
       <c r="M27" s="4" t="s">
@@ -5009,8 +5018,8 @@
       <c r="O27" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="P27"/>
-      <c r="Q27" s="4" t="s">
+      <c r="R27"/>
+      <c r="S27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD27" s="4" t="s">
@@ -5050,7 +5059,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L28"/>
       <c r="M28" s="4" t="s">
@@ -5059,10 +5068,10 @@
       <c r="N28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P28" s="4" t="s">
+      <c r="R28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q28" s="4" t="s">
+      <c r="S28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD28" s="4" t="s">
@@ -5104,7 +5113,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L29"/>
       <c r="M29" s="4" t="s">
@@ -5113,10 +5122,10 @@
       <c r="N29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P29" s="4" t="s">
+      <c r="R29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q29" s="4" t="s">
+      <c r="S29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD29" s="4" t="s">
@@ -5158,7 +5167,7 @@
         <v>14</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L30"/>
       <c r="M30" s="4" t="s">
@@ -5167,10 +5176,10 @@
       <c r="N30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P30" s="4" t="s">
+      <c r="R30" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q30" s="4" t="s">
+      <c r="S30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD30" s="4" t="s">
@@ -5212,7 +5221,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L31"/>
       <c r="M31" s="4" t="s">
@@ -5221,11 +5230,17 @@
       <c r="N31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="R31" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Q31" s="4" t="s">
+      <c r="S31" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA31" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="AB31" s="4" t="s">
         <v>76</v>
@@ -5269,7 +5284,7 @@
         <v>14</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>16</v>
@@ -5277,7 +5292,7 @@
       <c r="N32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q32" s="4" t="s">
+      <c r="S32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD32" s="4" t="s">
@@ -5316,7 +5331,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>16</v>
@@ -5324,7 +5339,7 @@
       <c r="N33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q33" s="4" t="s">
+      <c r="S33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD33" s="4" t="s">
@@ -5363,7 +5378,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>16</v>
@@ -5374,7 +5389,7 @@
       <c r="O34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Q34" s="4" t="s">
+      <c r="S34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD34" s="4" t="s">
@@ -5413,7 +5428,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>16</v>
@@ -5424,7 +5439,7 @@
       <c r="O35" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Q35" s="4" t="s">
+      <c r="S35" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD35" s="4" t="s">
@@ -5463,7 +5478,7 @@
         <v>14</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>16</v>
@@ -5474,7 +5489,7 @@
       <c r="O36" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Q36" s="4" t="s">
+      <c r="S36" s="4" t="s">
         <v>90</v>
       </c>
       <c r="AD36" s="4" t="s">
@@ -5513,7 +5528,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L37"/>
       <c r="M37" s="4" t="s">
@@ -5522,7 +5537,7 @@
       <c r="N37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD37" s="4" t="s">
@@ -5561,7 +5576,7 @@
         <v>14</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L38"/>
       <c r="M38" s="4" t="s">
@@ -5570,7 +5585,7 @@
       <c r="N38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q38" s="4" t="s">
+      <c r="S38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD38" s="4" t="s">
@@ -5609,7 +5624,7 @@
         <v>14</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L39"/>
       <c r="M39" s="4" t="s">
@@ -5618,7 +5633,7 @@
       <c r="N39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q39" s="4" t="s">
+      <c r="S39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD39" s="4" t="s">
@@ -5657,7 +5672,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L40"/>
       <c r="M40" s="4" t="s">
@@ -5666,7 +5681,7 @@
       <c r="N40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q40" s="4" t="s">
+      <c r="S40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD40" s="4" t="s">
@@ -5705,7 +5720,7 @@
         <v>14</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L41"/>
       <c r="M41" s="4" t="s">
@@ -5714,7 +5729,7 @@
       <c r="N41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q41" s="4" t="s">
+      <c r="S41" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD41" s="4" t="s">
@@ -5753,7 +5768,7 @@
         <v>14</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L42"/>
       <c r="M42" s="4" t="s">
@@ -5762,7 +5777,7 @@
       <c r="N42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q42" s="4" t="s">
+      <c r="S42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD42" s="4" t="s">
@@ -5801,7 +5816,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L43"/>
       <c r="M43" s="4" t="s">
@@ -5810,7 +5825,7 @@
       <c r="N43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q43" s="4" t="s">
+      <c r="S43" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD43" s="4" t="s">
@@ -5849,7 +5864,7 @@
         <v>14</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L44"/>
       <c r="M44" s="4" t="s">
@@ -5858,7 +5873,7 @@
       <c r="N44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q44" s="4" t="s">
+      <c r="S44" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD44" s="4" t="s">
@@ -5897,7 +5912,7 @@
         <v>14</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L45"/>
       <c r="M45" s="4" t="s">
@@ -5906,7 +5921,7 @@
       <c r="N45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q45" s="4" t="s">
+      <c r="S45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD45" s="4" t="s">
@@ -5945,7 +5960,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L46"/>
       <c r="M46" s="4" t="s">
@@ -5954,7 +5969,7 @@
       <c r="N46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q46" s="4" t="s">
+      <c r="S46" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD46" s="4" t="s">
@@ -5993,7 +6008,7 @@
         <v>14</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L47"/>
       <c r="M47" s="4" t="s">
@@ -6005,10 +6020,10 @@
       <c r="O47" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="P47" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Q47" s="4" t="s">
+      <c r="S47" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD47" s="4" t="s">
@@ -6050,7 +6065,7 @@
         <v>14</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L48"/>
       <c r="M48" s="4" t="s">
@@ -6062,7 +6077,7 @@
       <c r="O48" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q48" s="4" t="s">
+      <c r="S48" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD48" s="4" t="s">
@@ -6101,7 +6116,7 @@
         <v>14</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L49"/>
       <c r="M49" s="4" t="s">
@@ -6113,7 +6128,7 @@
       <c r="O49" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q49" s="4" t="s">
+      <c r="S49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD49" s="4" t="s">
@@ -6152,7 +6167,7 @@
         <v>14</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L50"/>
       <c r="M50" s="4" t="s">
@@ -6164,7 +6179,7 @@
       <c r="O50" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q50" s="4" t="s">
+      <c r="S50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD50" s="4" t="s">
@@ -6203,7 +6218,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L51"/>
       <c r="M51" s="4" t="s">
@@ -6215,7 +6230,7 @@
       <c r="O51" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q51" s="4" t="s">
+      <c r="S51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD51" s="4" t="s">
@@ -6254,7 +6269,7 @@
         <v>14</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L52"/>
       <c r="M52" s="4" t="s">
@@ -6266,7 +6281,7 @@
       <c r="O52" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q52" s="4" t="s">
+      <c r="S52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD52" s="4" t="s">
@@ -6305,7 +6320,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L53"/>
       <c r="M53" s="4" t="s">
@@ -6317,7 +6332,7 @@
       <c r="O53" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q53" s="4" t="s">
+      <c r="S53" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD53" s="4" t="s">
@@ -6356,7 +6371,7 @@
         <v>14</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L54"/>
       <c r="M54" s="4" t="s">
@@ -6368,7 +6383,7 @@
       <c r="O54" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q54" s="4" t="s">
+      <c r="S54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD54" s="4" t="s">
@@ -6407,7 +6422,7 @@
         <v>14</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L55"/>
       <c r="M55" s="4" t="s">
@@ -6419,7 +6434,7 @@
       <c r="O55" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q55" s="4" t="s">
+      <c r="S55" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD55" s="4" t="s">
@@ -6458,7 +6473,7 @@
         <v>14</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L56"/>
       <c r="M56" s="4" t="s">
@@ -6470,7 +6485,7 @@
       <c r="O56" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q56" s="4" t="s">
+      <c r="S56" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD56" s="4" t="s">
@@ -6509,7 +6524,7 @@
         <v>14</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L57"/>
       <c r="M57" s="4" t="s">
@@ -6521,7 +6536,7 @@
       <c r="O57" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="Q57" s="4" t="s">
+      <c r="S57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD57" s="4" t="s">
@@ -6560,7 +6575,7 @@
         <v>14</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L58"/>
       <c r="M58" s="4" t="s">
@@ -6572,7 +6587,7 @@
       <c r="O58" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="Q58" s="4" t="s">
+      <c r="S58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD58" s="4" t="s">
@@ -6614,7 +6629,7 @@
         <v>14</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L59"/>
       <c r="M59" s="4" t="s">
@@ -6623,8 +6638,14 @@
       <c r="N59" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q59" s="4" t="s">
+      <c r="S59" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="Z59" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA59" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="AB59" s="4" t="s">
         <v>133</v>
@@ -6665,7 +6686,7 @@
         <v>14</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L60"/>
       <c r="M60" s="4" t="s">
@@ -6677,7 +6698,7 @@
       <c r="O60" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="Q60" s="4" t="s">
+      <c r="S60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD60" s="4" t="s">
@@ -6716,7 +6737,7 @@
         <v>14</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L61"/>
       <c r="M61" s="4" t="s">
@@ -6728,7 +6749,7 @@
       <c r="O61" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="Q61" s="4" t="s">
+      <c r="S61" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD61" s="4" t="s">
@@ -6767,7 +6788,7 @@
         <v>14</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>16</v>
@@ -6778,7 +6799,7 @@
       <c r="O62" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="Q62" s="4" t="s">
+      <c r="S62" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD62" s="4" t="s">
@@ -6817,7 +6838,7 @@
         <v>14</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>16</v>
@@ -6828,7 +6849,7 @@
       <c r="O63" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="Q63" s="4" t="s">
+      <c r="S63" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AD63" s="4" t="s">
@@ -6867,7 +6888,7 @@
         <v>14</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>16</v>
@@ -6878,7 +6899,7 @@
       <c r="O64" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="Q64" s="4" t="s">
+      <c r="S64" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y64" s="4">

</xml_diff>

<commit_message>
entering more HJ8, HJ7, HJ27. Adding location remarks to the criteria for assigning ass occ in part 3
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-27-occ-entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEF351-991D-FC46-8585-B0D959865859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031BFA37-13A2-F546-9222-20261CF482F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2475,7 +2475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="245">
   <si>
     <t>genus</t>
   </si>
@@ -3018,6 +3018,198 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>unsure what Mb and Ct are - likely trees but not sure which species</t>
+  </si>
+  <si>
+    <t>ledge up forest, Pseudotsuga menziesii [verts]? to ct with Quercus garryana, Mb, and small Arbutus</t>
+  </si>
+  <si>
+    <t>Elymus glaucus</t>
+  </si>
+  <si>
+    <t>Melica harfordii</t>
+  </si>
+  <si>
+    <t>Bromus sterilis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etc (underlined)after taxon name </t>
+  </si>
+  <si>
+    <t>Lonicera hispidula</t>
+  </si>
+  <si>
+    <t>Madia gra</t>
+  </si>
+  <si>
+    <t>Bromus st</t>
+  </si>
+  <si>
+    <t>Elym gla</t>
+  </si>
+  <si>
+    <t>Meli har</t>
+  </si>
+  <si>
+    <t>Vicia sativa</t>
+  </si>
+  <si>
+    <t>Loni his</t>
+  </si>
+  <si>
+    <t>Vici sat</t>
+  </si>
+  <si>
+    <t>Sanicula crassicaulis</t>
+  </si>
+  <si>
+    <t>Sani cra</t>
+  </si>
+  <si>
+    <t>poly 48</t>
+  </si>
+  <si>
+    <t>next [grassy?], poly 48</t>
+  </si>
+  <si>
+    <t>Allium sps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromus sp. </t>
+  </si>
+  <si>
+    <t>with mixed [infolia]?</t>
+  </si>
+  <si>
+    <t>Selag wal</t>
+  </si>
+  <si>
+    <t>Racomitrium canescens</t>
+  </si>
+  <si>
+    <t>Collinsia p</t>
+  </si>
+  <si>
+    <t>poly 37</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland with clumps of Pseudotsuga menziesii</t>
+  </si>
+  <si>
+    <t>poly 52</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland</t>
+  </si>
+  <si>
+    <t>Cynosurus cristatus</t>
+  </si>
+  <si>
+    <t>Cyno cris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first seen abundant </t>
+  </si>
+  <si>
+    <t>Festuca rubra</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland, mostly under trees</t>
+  </si>
+  <si>
+    <t>Sinapis arvensis</t>
+  </si>
+  <si>
+    <t>Lychnis coronaria</t>
+  </si>
+  <si>
+    <t>Lych cor</t>
+  </si>
+  <si>
+    <t>Silene coronaria</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland, under trees</t>
+  </si>
+  <si>
+    <t>Luzu cam</t>
+  </si>
+  <si>
+    <t>Luzula campestris</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland, under oaks</t>
+  </si>
+  <si>
+    <t>Cyst fra</t>
+  </si>
+  <si>
+    <t>Cystopteris fragilis</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland, foot of shaded cliffs</t>
+  </si>
+  <si>
+    <t>Heuc mic</t>
+  </si>
+  <si>
+    <t>Heuchera micrantha</t>
+  </si>
+  <si>
+    <t>Quercus garryana woodland, ridge top</t>
+  </si>
+  <si>
+    <t>[Mohr]? mac</t>
+  </si>
+  <si>
+    <t>cannot decipher taxon name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galiano Island; Mount Sutil </t>
+  </si>
+  <si>
+    <t>plot 01</t>
+  </si>
+  <si>
+    <t>Cyti sco</t>
+  </si>
+  <si>
+    <t>Cytisus scoparius</t>
+  </si>
+  <si>
+    <t>Brom sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question mark next to taxon name Bromus sp. </t>
+  </si>
+  <si>
+    <t>Bromus c.f.</t>
+  </si>
+  <si>
+    <t>Eryth ore</t>
+  </si>
+  <si>
+    <t>Erythronium oregonum</t>
+  </si>
+  <si>
+    <t>Allium acuminatum</t>
+  </si>
+  <si>
+    <t>Luzula multiflora</t>
+  </si>
+  <si>
+    <t>Ramu occi</t>
+  </si>
+  <si>
+    <t>Ranunculus occidentalis</t>
+  </si>
+  <si>
+    <t>Cera arv</t>
+  </si>
+  <si>
+    <t>Cerastium arvense</t>
   </si>
 </sst>
 </file>
@@ -3159,7 +3351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3180,6 +3372,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3501,12 +3696,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AF64"/>
+  <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="137" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="AB31" sqref="AB31"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6909,6 +7104,1564 @@
         <v>18</v>
       </c>
     </row>
+    <row r="65" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <v>4</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G65" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R65" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF65" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>4</v>
+      </c>
+      <c r="B66" s="4">
+        <v>2</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G66" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R66" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF66" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <v>4</v>
+      </c>
+      <c r="B67" s="4">
+        <v>3</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G67" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R67" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB67" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF67" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>4</v>
+      </c>
+      <c r="B68" s="4">
+        <v>4</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R68" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF68" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>4</v>
+      </c>
+      <c r="B69" s="4">
+        <v>5</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R69" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF69" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <v>4</v>
+      </c>
+      <c r="B70" s="4">
+        <v>6</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G70" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R70" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF70" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>4</v>
+      </c>
+      <c r="B71" s="4">
+        <v>7</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O71" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R71" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF71" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>4</v>
+      </c>
+      <c r="B72" s="4">
+        <v>8</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G72" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R72" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF72" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>4</v>
+      </c>
+      <c r="B73" s="4">
+        <v>9</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G73" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R73" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB73" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF73" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>4</v>
+      </c>
+      <c r="B74" s="4">
+        <v>10</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G74" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O74" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R74" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF74" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>4</v>
+      </c>
+      <c r="B75" s="4">
+        <v>11</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G75" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R75" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF75" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>4</v>
+      </c>
+      <c r="B76" s="4">
+        <v>12</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G76" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R76" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF76" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>4</v>
+      </c>
+      <c r="B77" s="4">
+        <v>13</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G77" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R77" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF77" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>4</v>
+      </c>
+      <c r="B78" s="4">
+        <v>14</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G78" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="R78" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF78" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>4</v>
+      </c>
+      <c r="B79" s="4">
+        <v>15</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G79" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="R79" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>4</v>
+      </c>
+      <c r="B80" s="4">
+        <v>16</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G80" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="R80" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>4</v>
+      </c>
+      <c r="B81" s="4">
+        <v>17</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G81" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="R81" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB81" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>4</v>
+      </c>
+      <c r="B82" s="4">
+        <v>18</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G82" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="R82" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>5</v>
+      </c>
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G83" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R83" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>5</v>
+      </c>
+      <c r="B84" s="4">
+        <v>2</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G84" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O84" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R84" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>5</v>
+      </c>
+      <c r="B85" s="4">
+        <v>3</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G85" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O85" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R85" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>5</v>
+      </c>
+      <c r="B86" s="4">
+        <v>4</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G86" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R86" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>5</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G87" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="R87" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>5</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G88" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="R88" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>5</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G89" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O89" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="R89" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>5</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G90" s="4">
+        <v>20040312</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="R90" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF90" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>5</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G91" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K91" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R91" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y91" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>5</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G92" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R92" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y92" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>5</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G93" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R93" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y93" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>5</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G94" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="R94" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB94" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>5</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G95" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R95" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y95" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>5</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G96" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R96" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y96" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>5</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G97" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R97" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y97" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <v>5</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G98" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R98" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y98" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <v>5</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G99" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R99" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y99" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>5</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G100" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R100" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y100" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="4">
+        <v>5</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J101" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K101" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R101" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y101" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="4">
+        <v>5</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G102" s="4">
+        <v>20040324</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R102" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y102" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>